<commit_message>
Chatbot respondiendo inicialmente con las preguntas encontradas en la búsqueda semántica a partir de una consulta
</commit_message>
<xml_diff>
--- a/docs/documentos_entregables/Cronograma_proyecto_chatbot_discord_UTN.xlsx
+++ b/docs/documentos_entregables/Cronograma_proyecto_chatbot_discord_UTN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Downloads\documentos_entregables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lourd\Downloads\discord-chatbot\docs\documentos_entregables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92508012-25FB-4DA0-B6EE-9FDDC31A1D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AA884A-44E9-452A-B0B9-230009C2D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1105,7 +1105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1130,17 +1130,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1150,6 +1139,24 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1199,7 +1206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1213,18 +1220,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1442,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2548,7 +2556,7 @@
       <c r="A65" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="8" t="s">
         <v>196</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2565,7 +2573,7 @@
       <c r="A66" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="9" t="s">
         <v>200</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -2582,7 +2590,7 @@
       <c r="A67" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="9" t="s">
         <v>203</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -2599,7 +2607,7 @@
       <c r="A68" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="9" t="s">
         <v>207</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -2616,7 +2624,7 @@
       <c r="A69" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B69" s="9" t="s">
         <v>210</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -2633,7 +2641,7 @@
       <c r="A70" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="8" t="s">
         <v>212</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -3075,16 +3083,16 @@
       <c r="A96" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D96" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="E96" s="11" t="s">
         <v>287</v>
       </c>
     </row>
@@ -3092,16 +3100,16 @@
       <c r="A97" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B97" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D97" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="E97" s="11" t="s">
         <v>291</v>
       </c>
     </row>
@@ -3109,16 +3117,16 @@
       <c r="A98" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B98" s="6" t="s">
+      <c r="B98" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="D98" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="E98" s="11" t="s">
         <v>287</v>
       </c>
     </row>
@@ -3126,16 +3134,16 @@
       <c r="A99" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B99" s="6" t="s">
+      <c r="B99" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D99" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="E99" s="11" t="s">
         <v>296</v>
       </c>
     </row>
@@ -3143,16 +3151,16 @@
       <c r="A100" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="B100" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D100" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="E100" s="11" t="s">
         <v>299</v>
       </c>
     </row>
@@ -3160,16 +3168,16 @@
       <c r="A101" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B101" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="11" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3177,16 +3185,16 @@
       <c r="A102" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B102" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D102" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="E102" s="11" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3194,16 +3202,16 @@
       <c r="A103" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="B103" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="D103" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="E103" s="11" t="s">
         <v>308</v>
       </c>
     </row>
@@ -3211,16 +3219,16 @@
       <c r="A104" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B104" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="E104" s="2" t="s">
+      <c r="E104" s="11" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3228,16 +3236,16 @@
       <c r="A105" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D105" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="E105" s="2" t="s">
+      <c r="E105" s="11" t="s">
         <v>265</v>
       </c>
     </row>
@@ -3245,16 +3253,16 @@
       <c r="A106" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B106" s="6" t="s">
+      <c r="B106" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="E106" s="2" t="s">
+      <c r="E106" s="11" t="s">
         <v>265</v>
       </c>
     </row>

</xml_diff>